<commit_message>
Batch 42 Dec 10 2018
</commit_message>
<xml_diff>
--- a/Source Calibration Check.xlsx
+++ b/Source Calibration Check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="-15" windowWidth="12030" windowHeight="15180" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="11985" yWindow="-15" windowWidth="12030" windowHeight="15180" firstSheet="5" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="18th December 2008" sheetId="6" r:id="rId1"/>
@@ -19,10 +19,12 @@
     <sheet name="Dec 16 2013" sheetId="16" r:id="rId10"/>
     <sheet name="Sept 5 2014" sheetId="17" r:id="rId11"/>
     <sheet name="Sept 7 2017" sheetId="18" r:id="rId12"/>
+    <sheet name="Dec 10 2018" sheetId="19" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'18th December 2008'!$A$1:$F$12</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'4th  Feb 2010'!$A$1:$F$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="12">'Dec 10 2018'!$A$1:$H$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">'Dec 16 2013'!$A$1:$H$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Dec 2 2011'!$A$1:$H$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'December 6 2010'!$A$1:$F$30</definedName>
@@ -184,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="53">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -579,6 +581,9 @@
   </si>
   <si>
     <t>CCSEO Batch No.: 27</t>
+  </si>
+  <si>
+    <t>CCSEO Batch No.: 42</t>
   </si>
 </sst>
 </file>
@@ -2885,6 +2890,388 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" style="87" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="87" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="87" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="87" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="87" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="87" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="87" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="87"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="137" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="117"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="116" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="76">
+        <v>42970.168749999997</v>
+      </c>
+      <c r="C4" s="115" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="133" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="133"/>
+      <c r="F4" s="134"/>
+    </row>
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="97" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="108" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="108"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="114">
+        <f>B4-(6/24)</f>
+        <v>42969.918749999997</v>
+      </c>
+      <c r="F5" s="113" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="77">
+        <v>455.5</v>
+      </c>
+      <c r="C6" s="105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="78">
+        <f>B6*110</f>
+        <v>50105</v>
+      </c>
+      <c r="E6" s="112" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="111"/>
+    </row>
+    <row r="7" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="98"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="110" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="91"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="103" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="109" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="135">
+        <v>42985.6875</v>
+      </c>
+      <c r="D8" s="135"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="84">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="100"/>
+      <c r="B9" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="79">
+        <f>H10</f>
+        <v>1.0110416389517094</v>
+      </c>
+      <c r="D9" s="108"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="97" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="85">
+        <v>751.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="100"/>
+      <c r="B10" s="98" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="80">
+        <v>1.0005999999999999</v>
+      </c>
+      <c r="D10" s="108"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="107" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="86">
+        <f>((H8+273)*760)/(H9*295)</f>
+        <v>1.0110416389517094</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="100"/>
+      <c r="B11" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="81">
+        <v>463.1</v>
+      </c>
+      <c r="D11" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="95"/>
+      <c r="F11" s="89"/>
+      <c r="H11" s="91"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="100"/>
+      <c r="B12" s="98" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="82">
+        <v>-91.260999999999996</v>
+      </c>
+      <c r="D12" s="87" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="95"/>
+      <c r="F12" s="89"/>
+      <c r="H12" s="91"/>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="98"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="83">
+        <f>-C12*C11*C10*C9</f>
+        <v>42755.259318756951</v>
+      </c>
+      <c r="E13" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="89"/>
+      <c r="H13" s="91"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="100"/>
+      <c r="B14" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="99">
+        <f>EXP(-0.693*(C8-E5)/73.831)</f>
+        <v>0.86242228695676859</v>
+      </c>
+      <c r="D14" s="98"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="89"/>
+      <c r="H14" s="91"/>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="98"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="83">
+        <f>B6*C14*110</f>
+        <v>43211.668687968893</v>
+      </c>
+      <c r="E15" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="89"/>
+      <c r="H15" s="91"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="94"/>
+      <c r="B16" s="106"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="74">
+        <f>(D13-D15)/D13*100</f>
+        <v>-1.0674929271489955</v>
+      </c>
+      <c r="E16" s="92" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="89"/>
+      <c r="H16" s="91"/>
+    </row>
+    <row r="17" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="98"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="89"/>
+      <c r="H17" s="91"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="136">
+        <f>C8</f>
+        <v>42985.6875</v>
+      </c>
+      <c r="D18" s="136"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="89"/>
+      <c r="H18" s="91"/>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="97" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="98"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="81">
+        <v>43230</v>
+      </c>
+      <c r="E19" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="89"/>
+      <c r="H19" s="91"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="100"/>
+      <c r="B20" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="99">
+        <f>EXP(-0.693*(C18-E5)/73.831)</f>
+        <v>0.86242228695676859</v>
+      </c>
+      <c r="D20" s="98"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="89"/>
+      <c r="H20" s="91"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="96"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="83">
+        <f>B6*C20*110</f>
+        <v>43211.668687968893</v>
+      </c>
+      <c r="E21" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="89"/>
+      <c r="H21" s="91"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="94"/>
+      <c r="B22" s="93"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="74">
+        <f>(D19-D21)/D19*100</f>
+        <v>4.2404145341445265E-2</v>
+      </c>
+      <c r="E22" s="92" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="89"/>
+      <c r="H22" s="91"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F23" s="89"/>
+      <c r="H23" s="91"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24" s="89"/>
+      <c r="H24" s="91"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="90"/>
+      <c r="C27" s="89"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="88"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="88"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C18:D18"/>
+  </mergeCells>
+  <pageMargins left="0.99" right="0.4" top="0.96" bottom="0.71" header="0.25" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
@@ -2923,7 +3310,7 @@
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" s="118"/>
       <c r="C3" s="118"/>
@@ -2936,7 +3323,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="76">
-        <v>42970.168749999997</v>
+        <v>43431.072916666664</v>
       </c>
       <c r="C4" s="115" t="s">
         <v>19</v>
@@ -2958,7 +3345,7 @@
       <c r="D5" s="96"/>
       <c r="E5" s="114">
         <f>B4-(6/24)</f>
-        <v>42969.918749999997</v>
+        <v>43430.822916666664</v>
       </c>
       <c r="F5" s="113" t="s">
         <v>20</v>
@@ -2969,14 +3356,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="77">
-        <v>455.5</v>
+        <v>383.8</v>
       </c>
       <c r="C6" s="105" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="78">
         <f>B6*110</f>
-        <v>50105</v>
+        <v>42218</v>
       </c>
       <c r="E6" s="112" t="s">
         <v>9</v>
@@ -3002,7 +3389,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="135">
-        <v>42985.6875</v>
+        <v>43444.620138888888</v>
       </c>
       <c r="D8" s="135"/>
       <c r="E8" s="101"/>
@@ -3011,7 +3398,7 @@
         <v>39</v>
       </c>
       <c r="H8" s="84">
-        <v>22</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -3021,7 +3408,7 @@
       </c>
       <c r="C9" s="79">
         <f>H10</f>
-        <v>1.0110416389517094</v>
+        <v>0.99643760923997882</v>
       </c>
       <c r="D9" s="108"/>
       <c r="E9" s="95"/>
@@ -3030,7 +3417,7 @@
         <v>40</v>
       </c>
       <c r="H9" s="85">
-        <v>751.7</v>
+        <v>762.2</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3039,7 +3426,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="80">
-        <v>1.0005999999999999</v>
+        <v>1.0008999999999999</v>
       </c>
       <c r="D10" s="108"/>
       <c r="E10" s="95"/>
@@ -3049,7 +3436,7 @@
       </c>
       <c r="H10" s="86">
         <f>((H8+273)*760)/(H9*295)</f>
-        <v>1.0110416389517094</v>
+        <v>0.99643760923997882</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3058,7 +3445,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="81">
-        <v>463.1</v>
+        <v>462.1</v>
       </c>
       <c r="D11" s="104" t="s">
         <v>34</v>
@@ -3073,7 +3460,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="82">
-        <v>-91.260999999999996</v>
+        <v>-80.367999999999995</v>
       </c>
       <c r="D12" s="87" t="s">
         <v>27</v>
@@ -3090,7 +3477,7 @@
       <c r="C13" s="89"/>
       <c r="D13" s="83">
         <f>-C12*C11*C10*C9</f>
-        <v>42755.259318756951</v>
+        <v>37039.057721149569</v>
       </c>
       <c r="E13" s="95" t="s">
         <v>9</v>
@@ -3105,7 +3492,7 @@
       </c>
       <c r="C14" s="99">
         <f>EXP(-0.693*(C8-E5)/73.831)</f>
-        <v>0.86242228695676859</v>
+        <v>0.87853029874190103</v>
       </c>
       <c r="D14" s="98"/>
       <c r="E14" s="95"/>
@@ -3120,7 +3507,7 @@
       <c r="C15" s="89"/>
       <c r="D15" s="83">
         <f>B6*C14*110</f>
-        <v>43211.668687968893</v>
+        <v>37089.792152285576</v>
       </c>
       <c r="E15" s="95" t="s">
         <v>9</v>
@@ -3134,7 +3521,7 @@
       <c r="C16" s="105"/>
       <c r="D16" s="74">
         <f>(D13-D15)/D13*100</f>
-        <v>-1.0674929271489955</v>
+        <v>-0.13697549089386493</v>
       </c>
       <c r="E16" s="92" t="s">
         <v>28</v>
@@ -3159,7 +3546,7 @@
       </c>
       <c r="C18" s="136">
         <f>C8</f>
-        <v>42985.6875</v>
+        <v>43444.620138888888</v>
       </c>
       <c r="D18" s="136"/>
       <c r="E18" s="101"/>
@@ -3173,7 +3560,7 @@
       <c r="B19" s="98"/>
       <c r="C19" s="89"/>
       <c r="D19" s="81">
-        <v>43230</v>
+        <v>37092</v>
       </c>
       <c r="E19" s="95" t="s">
         <v>9</v>
@@ -3188,7 +3575,7 @@
       </c>
       <c r="C20" s="99">
         <f>EXP(-0.693*(C18-E5)/73.831)</f>
-        <v>0.86242228695676859</v>
+        <v>0.87853029874190103</v>
       </c>
       <c r="D20" s="98"/>
       <c r="E20" s="95"/>
@@ -3203,7 +3590,7 @@
       <c r="C21" s="89"/>
       <c r="D21" s="83">
         <f>B6*C20*110</f>
-        <v>43211.668687968893</v>
+        <v>37089.792152285576</v>
       </c>
       <c r="E21" s="95" t="s">
         <v>9</v>
@@ -3217,7 +3604,7 @@
       <c r="C22" s="93"/>
       <c r="D22" s="74">
         <f>(D19-D21)/D19*100</f>
-        <v>4.2404145341445265E-2</v>
+        <v>5.9523555333336926E-3</v>
       </c>
       <c r="E22" s="92" t="s">
         <v>28</v>

</xml_diff>